<commit_message>
Ajustes tildes mensaje creación de usuarios, nombre de usuario en mayuscula
</commit_message>
<xml_diff>
--- a/docs/EVAC_ Matriz de Pruebas definitivos.xlsx
+++ b/docs/EVAC_ Matriz de Pruebas definitivos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="720" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="720"/>
   </bookViews>
   <sheets>
     <sheet name="Perfil Fuente" sheetId="1" r:id="rId1"/>
@@ -4558,6 +4558,90 @@
     <xf numFmtId="0" fontId="27" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4576,101 +4660,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5554,10 +5554,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N133"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A68" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A121" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A36" sqref="A36"/>
-      <selection pane="topRight" activeCell="L105" sqref="L105:L110"/>
+      <selection pane="topRight" activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5580,13 +5580,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111"/>
-      <c r="B1" s="112" t="s">
+      <c r="A1" s="139"/>
+      <c r="B1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -5598,11 +5598,11 @@
       <c r="N1"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="111"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="A2" s="139"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
@@ -5616,11 +5616,11 @@
       <c r="N2"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="111"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
+      <c r="A3" s="139"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
       <c r="F3" s="6" t="s">
         <v>2</v>
       </c>
@@ -5634,11 +5634,11 @@
       <c r="N3"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
       <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
@@ -5652,11 +5652,11 @@
       <c r="N4"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="111"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
+      <c r="A5" s="139"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140"/>
       <c r="F5" s="6"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -5668,11 +5668,11 @@
       <c r="N5"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="111"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
+      <c r="A6" s="139"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
       <c r="F6" s="7"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -5688,14 +5688,14 @@
         <v>4</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113" t="s">
+      <c r="D7" s="141"/>
+      <c r="E7" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="113"/>
+      <c r="F7" s="141"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="4"/>
@@ -5706,12 +5706,12 @@
       <c r="N7"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="4"/>
@@ -5722,12 +5722,12 @@
       <c r="N8"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="114"/>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
+      <c r="A9" s="142"/>
+      <c r="B9" s="142"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="4"/>
@@ -5738,14 +5738,14 @@
       <c r="N9"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="115" t="s">
+      <c r="A10" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="115"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
+      <c r="B10" s="143"/>
+      <c r="C10" s="143"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="143"/>
+      <c r="F10" s="143"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="4"/>
@@ -5756,14 +5756,14 @@
       <c r="N10"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="116"/>
-      <c r="C11" s="116"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
+      <c r="B11" s="144"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="144"/>
+      <c r="F11" s="144"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="4"/>
@@ -5774,14 +5774,14 @@
       <c r="N11"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
+      <c r="B12" s="144"/>
+      <c r="C12" s="144"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="144"/>
+      <c r="F12" s="144"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="4"/>
@@ -5794,14 +5794,14 @@
       <c r="N12"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="144"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="4"/>
@@ -5814,10 +5814,10 @@
       <c r="N13"/>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="117"/>
+      <c r="B14" s="129"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -5834,10 +5834,10 @@
       <c r="N14"/>
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="118"/>
+      <c r="B15" s="130"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -5854,10 +5854,10 @@
       <c r="N15"/>
     </row>
     <row r="16" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="119" t="s">
+      <c r="A16" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="119"/>
+      <c r="B16" s="131"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -5874,86 +5874,86 @@
       <c r="N16"/>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="120" t="s">
+      <c r="A17" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="121"/>
-      <c r="F17" s="121"/>
-      <c r="G17" s="121"/>
-      <c r="H17" s="121"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="121"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="133"/>
+      <c r="I17" s="133"/>
+      <c r="J17" s="133"/>
       <c r="K17" s="19"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17"/>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="122"/>
-      <c r="C18" s="123"/>
-      <c r="D18" s="123"/>
-      <c r="E18" s="123"/>
-      <c r="F18" s="123"/>
-      <c r="G18" s="123"/>
-      <c r="H18" s="123"/>
-      <c r="I18" s="123"/>
-      <c r="J18" s="123"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="135"/>
+      <c r="D18" s="135"/>
+      <c r="E18" s="135"/>
+      <c r="F18" s="135"/>
+      <c r="G18" s="135"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="135"/>
+      <c r="J18" s="135"/>
       <c r="K18" s="20"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
       <c r="N18"/>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="124" t="s">
+      <c r="A19" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="125" t="s">
+      <c r="B19" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="125" t="s">
+      <c r="C19" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="124" t="s">
+      <c r="D19" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="124" t="s">
+      <c r="E19" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="124" t="s">
+      <c r="F19" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="126" t="s">
+      <c r="G19" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="126"/>
-      <c r="I19" s="126"/>
-      <c r="J19" s="125" t="s">
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="137" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="127" t="s">
+      <c r="K19" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="128" t="s">
+      <c r="L19" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="M19" s="128" t="s">
+      <c r="M19" s="126" t="s">
         <v>31</v>
       </c>
       <c r="N19"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="124"/>
-      <c r="B20" s="125"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="124"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="124"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="136"/>
       <c r="G20" s="22" t="s">
         <v>32</v>
       </c>
@@ -5963,10 +5963,10 @@
       <c r="I20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="125"/>
-      <c r="K20" s="127"/>
-      <c r="L20" s="128"/>
-      <c r="M20" s="128"/>
+      <c r="J20" s="137"/>
+      <c r="K20" s="125"/>
+      <c r="L20" s="126"/>
+      <c r="M20" s="126"/>
       <c r="N20"/>
     </row>
     <row r="21" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
@@ -5998,24 +5998,24 @@
       <c r="N21"/>
     </row>
     <row r="22" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="129" t="s">
+      <c r="A22" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="129"/>
-      <c r="C22" s="129"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="129"/>
-      <c r="F22" s="129"/>
-      <c r="G22" s="129"/>
-      <c r="H22" s="129"/>
-      <c r="I22" s="129"/>
-      <c r="J22" s="129"/>
+      <c r="B22" s="127"/>
+      <c r="C22" s="127"/>
+      <c r="D22" s="127"/>
+      <c r="E22" s="127"/>
+      <c r="F22" s="127"/>
+      <c r="G22" s="127"/>
+      <c r="H22" s="127"/>
+      <c r="I22" s="127"/>
+      <c r="J22" s="127"/>
       <c r="K22" s="30"/>
       <c r="L22" s="31"/>
       <c r="M22" s="31"/>
       <c r="N22"/>
     </row>
-    <row r="23" spans="1:14" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="32" t="s">
         <v>42</v>
       </c>
@@ -6051,7 +6051,7 @@
       </c>
       <c r="N23" s="37"/>
     </row>
-    <row r="24" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>42</v>
       </c>
@@ -6085,7 +6085,7 @@
       <c r="M24" s="36"/>
       <c r="N24" s="37"/>
     </row>
-    <row r="25" spans="1:14" ht="140.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="140.25" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>42</v>
       </c>
@@ -6117,7 +6117,7 @@
       <c r="M25" s="36"/>
       <c r="N25" s="37"/>
     </row>
-    <row r="26" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>58</v>
       </c>
@@ -6147,7 +6147,7 @@
       <c r="M26" s="36"/>
       <c r="N26" s="37"/>
     </row>
-    <row r="27" spans="1:14" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="s">
         <v>61</v>
       </c>
@@ -6179,7 +6179,7 @@
       <c r="M27" s="36"/>
       <c r="N27" s="37"/>
     </row>
-    <row r="28" spans="1:14" ht="76.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
         <v>66</v>
       </c>
@@ -6215,7 +6215,7 @@
       </c>
       <c r="N28" s="37"/>
     </row>
-    <row r="29" spans="1:14" ht="127.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>73</v>
       </c>
@@ -6255,7 +6255,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="127.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>81</v>
       </c>
@@ -6291,7 +6291,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="127.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>85</v>
       </c>
@@ -6327,7 +6327,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="127.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="127.5" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>89</v>
       </c>
@@ -6401,7 +6401,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="89.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
         <v>101</v>
       </c>
@@ -6441,7 +6441,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="89.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A35" s="32" t="s">
         <v>109</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="37" spans="1:14" ht="76.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" ht="76.5" x14ac:dyDescent="0.25">
       <c r="A37" s="32" t="s">
         <v>118</v>
       </c>
@@ -6551,7 +6551,7 @@
       <c r="M37" s="36"/>
       <c r="N37" s="37"/>
     </row>
-    <row r="38" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
         <v>122</v>
       </c>
@@ -6583,7 +6583,7 @@
       <c r="M38" s="36"/>
       <c r="N38" s="37"/>
     </row>
-    <row r="39" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A39" s="32" t="s">
         <v>126</v>
       </c>
@@ -6615,7 +6615,7 @@
       <c r="M39" s="36"/>
       <c r="N39" s="37"/>
     </row>
-    <row r="40" spans="1:14" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A40" s="32" t="s">
         <v>129</v>
       </c>
@@ -6649,7 +6649,7 @@
       <c r="M40" s="36"/>
       <c r="N40" s="37"/>
     </row>
-    <row r="41" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A41" s="32" t="s">
         <v>134</v>
       </c>
@@ -6685,7 +6685,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="42" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
         <v>139</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
         <v>143</v>
       </c>
@@ -6757,7 +6757,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
         <v>147</v>
       </c>
@@ -6789,7 +6789,7 @@
       <c r="M44" s="36"/>
       <c r="N44" s="37"/>
     </row>
-    <row r="45" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A45" s="32" t="s">
         <v>150</v>
       </c>
@@ -6821,7 +6821,7 @@
       <c r="M45" s="36"/>
       <c r="N45" s="37"/>
     </row>
-    <row r="46" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
         <v>153</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A47" s="32" t="s">
         <v>155</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
         <v>157</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A49" s="32" t="s">
         <v>159</v>
       </c>
@@ -6965,17 +6965,17 @@
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="130" t="s">
+    <row r="50" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="116" t="s">
         <v>161</v>
       </c>
-      <c r="B50" s="131" t="s">
+      <c r="B50" s="114" t="s">
         <v>162</v>
       </c>
       <c r="C50" s="33">
         <v>42594</v>
       </c>
-      <c r="D50" s="130" t="s">
+      <c r="D50" s="116" t="s">
         <v>163</v>
       </c>
       <c r="E50" s="32" t="s">
@@ -6989,7 +6989,7 @@
         <v>47</v>
       </c>
       <c r="I50" s="27"/>
-      <c r="J50" s="132" t="s">
+      <c r="J50" s="128" t="s">
         <v>48</v>
       </c>
       <c r="K50" s="50"/>
@@ -6997,13 +6997,13 @@
       <c r="M50" s="36"/>
       <c r="N50" s="54"/>
     </row>
-    <row r="51" spans="1:14" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="130"/>
-      <c r="B51" s="131"/>
+    <row r="51" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="116"/>
+      <c r="B51" s="114"/>
       <c r="C51" s="33">
         <v>42594</v>
       </c>
-      <c r="D51" s="130"/>
+      <c r="D51" s="116"/>
       <c r="E51" s="32" t="s">
         <v>166</v>
       </c>
@@ -7013,7 +7013,7 @@
       <c r="G51" s="26"/>
       <c r="H51" s="55"/>
       <c r="I51" s="27"/>
-      <c r="J51" s="132"/>
+      <c r="J51" s="128"/>
       <c r="K51" s="34" t="s">
         <v>49</v>
       </c>
@@ -7021,13 +7021,13 @@
       <c r="M51" s="36"/>
       <c r="N51" s="54"/>
     </row>
-    <row r="52" spans="1:14" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="130"/>
-      <c r="B52" s="131"/>
+    <row r="52" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="116"/>
+      <c r="B52" s="114"/>
       <c r="C52" s="33">
         <v>42594</v>
       </c>
-      <c r="D52" s="130"/>
+      <c r="D52" s="116"/>
       <c r="E52" s="32" t="s">
         <v>168</v>
       </c>
@@ -7037,7 +7037,7 @@
       <c r="G52" s="26"/>
       <c r="H52" s="55"/>
       <c r="I52" s="27"/>
-      <c r="J52" s="132"/>
+      <c r="J52" s="128"/>
       <c r="K52" s="34" t="s">
         <v>49</v>
       </c>
@@ -7045,13 +7045,13 @@
       <c r="M52" s="36"/>
       <c r="N52" s="54"/>
     </row>
-    <row r="53" spans="1:14" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="130"/>
-      <c r="B53" s="131"/>
+    <row r="53" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="116"/>
+      <c r="B53" s="114"/>
       <c r="C53" s="33">
         <v>42594</v>
       </c>
-      <c r="D53" s="130"/>
+      <c r="D53" s="116"/>
       <c r="E53" s="56" t="s">
         <v>170</v>
       </c>
@@ -7063,7 +7063,7 @@
         <v>47</v>
       </c>
       <c r="I53" s="27"/>
-      <c r="J53" s="132"/>
+      <c r="J53" s="128"/>
       <c r="K53" s="34" t="s">
         <v>49</v>
       </c>
@@ -7071,13 +7071,13 @@
       <c r="M53" s="36"/>
       <c r="N53" s="54"/>
     </row>
-    <row r="54" spans="1:14" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="130"/>
-      <c r="B54" s="131"/>
+    <row r="54" spans="1:14" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="116"/>
+      <c r="B54" s="114"/>
       <c r="C54" s="33">
         <v>42594</v>
       </c>
-      <c r="D54" s="130"/>
+      <c r="D54" s="116"/>
       <c r="E54" s="56" t="s">
         <v>172</v>
       </c>
@@ -7089,7 +7089,7 @@
         <v>47</v>
       </c>
       <c r="I54" s="27"/>
-      <c r="J54" s="132"/>
+      <c r="J54" s="128"/>
       <c r="K54" s="34" t="s">
         <v>174</v>
       </c>
@@ -7101,13 +7101,13 @@
         <v>176</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="130"/>
-      <c r="B55" s="131"/>
+    <row r="55" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="116"/>
+      <c r="B55" s="114"/>
       <c r="C55" s="33">
         <v>42594</v>
       </c>
-      <c r="D55" s="130"/>
+      <c r="D55" s="116"/>
       <c r="E55" s="32" t="s">
         <v>177</v>
       </c>
@@ -7119,7 +7119,7 @@
         <v>47</v>
       </c>
       <c r="I55" s="27"/>
-      <c r="J55" s="132"/>
+      <c r="J55" s="128"/>
       <c r="K55" s="34" t="s">
         <v>49</v>
       </c>
@@ -7127,13 +7127,13 @@
       <c r="M55" s="36"/>
       <c r="N55" s="54"/>
     </row>
-    <row r="56" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="130"/>
-      <c r="B56" s="131"/>
+    <row r="56" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A56" s="116"/>
+      <c r="B56" s="114"/>
       <c r="C56" s="33">
         <v>42594</v>
       </c>
-      <c r="D56" s="130"/>
+      <c r="D56" s="116"/>
       <c r="E56" s="32"/>
       <c r="F56" s="32" t="s">
         <v>179</v>
@@ -7155,13 +7155,13 @@
         <v>108</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="130"/>
-      <c r="B57" s="131"/>
+    <row r="57" spans="1:14" ht="51" x14ac:dyDescent="0.25">
+      <c r="A57" s="116"/>
+      <c r="B57" s="114"/>
       <c r="C57" s="33">
         <v>42594</v>
       </c>
-      <c r="D57" s="130"/>
+      <c r="D57" s="116"/>
       <c r="E57" s="32"/>
       <c r="F57" s="32" t="s">
         <v>180</v>
@@ -7185,17 +7185,17 @@
         <v>108</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="131" t="s">
+    <row r="58" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="114" t="s">
         <v>182</v>
       </c>
-      <c r="B58" s="131" t="s">
+      <c r="B58" s="114" t="s">
         <v>183</v>
       </c>
-      <c r="C58" s="133">
+      <c r="C58" s="115">
         <v>42598</v>
       </c>
-      <c r="D58" s="130" t="s">
+      <c r="D58" s="116" t="s">
         <v>184</v>
       </c>
       <c r="E58" s="32" t="s">
@@ -7222,10 +7222,10 @@
       </c>
     </row>
     <row r="59" spans="1:14" ht="63" x14ac:dyDescent="0.25">
-      <c r="A59" s="131"/>
-      <c r="B59" s="131"/>
-      <c r="C59" s="133"/>
-      <c r="D59" s="130"/>
+      <c r="A59" s="114"/>
+      <c r="B59" s="114"/>
+      <c r="C59" s="115"/>
+      <c r="D59" s="116"/>
       <c r="E59" s="32" t="s">
         <v>188</v>
       </c>
@@ -7249,11 +7249,11 @@
         <v>190</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="131"/>
-      <c r="B60" s="131"/>
-      <c r="C60" s="133"/>
-      <c r="D60" s="130"/>
+    <row r="60" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A60" s="114"/>
+      <c r="B60" s="114"/>
+      <c r="C60" s="115"/>
+      <c r="D60" s="116"/>
       <c r="E60" s="32" t="s">
         <v>191</v>
       </c>
@@ -7273,7 +7273,7 @@
       <c r="M60" s="36"/>
       <c r="N60" s="54"/>
     </row>
-    <row r="61" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
         <v>193</v>
       </c>
@@ -7307,7 +7307,7 @@
       <c r="M61" s="36"/>
       <c r="N61" s="54"/>
     </row>
-    <row r="62" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A62" s="32" t="s">
         <v>198</v>
       </c>
@@ -7346,19 +7346,19 @@
       </c>
     </row>
     <row r="63" spans="1:14" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="130" t="s">
+      <c r="A63" s="116" t="s">
         <v>205</v>
       </c>
-      <c r="B63" s="131" t="s">
+      <c r="B63" s="114" t="s">
         <v>206</v>
       </c>
-      <c r="C63" s="133">
+      <c r="C63" s="115">
         <v>42598</v>
       </c>
-      <c r="D63" s="131" t="s">
+      <c r="D63" s="114" t="s">
         <v>207</v>
       </c>
-      <c r="E63" s="131" t="s">
+      <c r="E63" s="114" t="s">
         <v>208</v>
       </c>
       <c r="F63" s="32" t="s">
@@ -7379,16 +7379,16 @@
       <c r="M63" s="29" t="s">
         <v>211</v>
       </c>
-      <c r="N63" s="134" t="s">
+      <c r="N63" s="113" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="64" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="A64" s="130"/>
-      <c r="B64" s="131"/>
-      <c r="C64" s="133"/>
-      <c r="D64" s="131"/>
-      <c r="E64" s="131"/>
+      <c r="A64" s="116"/>
+      <c r="B64" s="114"/>
+      <c r="C64" s="115"/>
+      <c r="D64" s="114"/>
+      <c r="E64" s="114"/>
       <c r="F64" s="32" t="s">
         <v>213</v>
       </c>
@@ -7407,7 +7407,7 @@
       <c r="M64" s="29" t="s">
         <v>214</v>
       </c>
-      <c r="N64" s="134"/>
+      <c r="N64" s="113"/>
     </row>
     <row r="65" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A65" s="52" t="s">
@@ -7447,8 +7447,8 @@
         <v>221</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="130" t="s">
+    <row r="66" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="116" t="s">
         <v>222</v>
       </c>
       <c r="B66" s="32" t="s">
@@ -7481,15 +7481,15 @@
       <c r="M66" s="36"/>
       <c r="N66" s="54"/>
     </row>
-    <row r="67" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="130"/>
-      <c r="B67" s="131" t="s">
+    <row r="67" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="116"/>
+      <c r="B67" s="114" t="s">
         <v>227</v>
       </c>
-      <c r="C67" s="135">
+      <c r="C67" s="119">
         <v>42598</v>
       </c>
-      <c r="D67" s="130" t="s">
+      <c r="D67" s="116" t="s">
         <v>228</v>
       </c>
       <c r="E67" s="62" t="s">
@@ -7514,10 +7514,10 @@
       <c r="N67" s="54"/>
     </row>
     <row r="68" spans="1:14" ht="63.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="130"/>
-      <c r="B68" s="131"/>
-      <c r="C68" s="135"/>
-      <c r="D68" s="130"/>
+      <c r="A68" s="116"/>
+      <c r="B68" s="114"/>
+      <c r="C68" s="119"/>
+      <c r="D68" s="116"/>
       <c r="E68" s="62" t="s">
         <v>231</v>
       </c>
@@ -7541,11 +7541,11 @@
         <v>233</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="130"/>
-      <c r="B69" s="131"/>
-      <c r="C69" s="135"/>
-      <c r="D69" s="130"/>
+    <row r="69" spans="1:14" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="116"/>
+      <c r="B69" s="114"/>
+      <c r="C69" s="119"/>
+      <c r="D69" s="116"/>
       <c r="E69" s="64" t="s">
         <v>234</v>
       </c>
@@ -7569,7 +7569,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A70" s="32" t="s">
         <v>236</v>
       </c>
@@ -7605,20 +7605,20 @@
         <v>187</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="131" t="s">
+    <row r="71" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="114" t="s">
         <v>239</v>
       </c>
-      <c r="B71" s="131" t="s">
+      <c r="B71" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="C71" s="133">
+      <c r="C71" s="115">
         <v>42599</v>
       </c>
-      <c r="D71" s="131" t="s">
+      <c r="D71" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="E71" s="131" t="s">
+      <c r="E71" s="114" t="s">
         <v>242</v>
       </c>
       <c r="F71" s="32" t="s">
@@ -7637,12 +7637,12 @@
       <c r="M71" s="36"/>
       <c r="N71" s="66"/>
     </row>
-    <row r="72" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="131"/>
-      <c r="B72" s="131"/>
-      <c r="C72" s="133"/>
-      <c r="D72" s="131"/>
-      <c r="E72" s="131"/>
+    <row r="72" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A72" s="114"/>
+      <c r="B72" s="114"/>
+      <c r="C72" s="115"/>
+      <c r="D72" s="114"/>
+      <c r="E72" s="114"/>
       <c r="F72" s="32" t="s">
         <v>244</v>
       </c>
@@ -7661,20 +7661,20 @@
       <c r="M72" s="36"/>
       <c r="N72" s="66"/>
     </row>
-    <row r="73" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="131" t="s">
+    <row r="73" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="114" t="s">
         <v>245</v>
       </c>
-      <c r="B73" s="131" t="s">
+      <c r="B73" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="C73" s="133">
+      <c r="C73" s="115">
         <v>42599</v>
       </c>
-      <c r="D73" s="131" t="s">
+      <c r="D73" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="E73" s="131" t="s">
+      <c r="E73" s="114" t="s">
         <v>246</v>
       </c>
       <c r="F73" s="32" t="s">
@@ -7693,12 +7693,12 @@
       <c r="M73" s="36"/>
       <c r="N73" s="66"/>
     </row>
-    <row r="74" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="131"/>
-      <c r="B74" s="131"/>
-      <c r="C74" s="133"/>
-      <c r="D74" s="131"/>
-      <c r="E74" s="131"/>
+    <row r="74" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A74" s="114"/>
+      <c r="B74" s="114"/>
+      <c r="C74" s="115"/>
+      <c r="D74" s="114"/>
+      <c r="E74" s="114"/>
       <c r="F74" s="32" t="s">
         <v>247</v>
       </c>
@@ -7717,20 +7717,20 @@
       <c r="M74" s="36"/>
       <c r="N74" s="66"/>
     </row>
-    <row r="75" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="131" t="s">
+    <row r="75" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="114" t="s">
         <v>248</v>
       </c>
-      <c r="B75" s="131" t="s">
+      <c r="B75" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="C75" s="133">
+      <c r="C75" s="115">
         <v>42599</v>
       </c>
-      <c r="D75" s="131" t="s">
+      <c r="D75" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="E75" s="131" t="s">
+      <c r="E75" s="114" t="s">
         <v>246</v>
       </c>
       <c r="F75" s="32" t="s">
@@ -7749,12 +7749,12 @@
       <c r="M75" s="36"/>
       <c r="N75" s="66"/>
     </row>
-    <row r="76" spans="1:14" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="131"/>
-      <c r="B76" s="131"/>
-      <c r="C76" s="133"/>
-      <c r="D76" s="131"/>
-      <c r="E76" s="131"/>
+    <row r="76" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="114"/>
+      <c r="B76" s="114"/>
+      <c r="C76" s="115"/>
+      <c r="D76" s="114"/>
+      <c r="E76" s="114"/>
       <c r="F76" s="32" t="s">
         <v>249</v>
       </c>
@@ -7771,20 +7771,20 @@
       <c r="M76" s="36"/>
       <c r="N76" s="66"/>
     </row>
-    <row r="77" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="131" t="s">
+    <row r="77" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="114" t="s">
         <v>250</v>
       </c>
-      <c r="B77" s="131" t="s">
+      <c r="B77" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="C77" s="133">
+      <c r="C77" s="115">
         <v>42599</v>
       </c>
-      <c r="D77" s="131" t="s">
+      <c r="D77" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="E77" s="131" t="s">
+      <c r="E77" s="114" t="s">
         <v>251</v>
       </c>
       <c r="F77" s="32" t="s">
@@ -7803,12 +7803,12 @@
       <c r="M77" s="36"/>
       <c r="N77" s="66"/>
     </row>
-    <row r="78" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="131"/>
-      <c r="B78" s="131"/>
-      <c r="C78" s="133"/>
-      <c r="D78" s="131"/>
-      <c r="E78" s="131"/>
+    <row r="78" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A78" s="114"/>
+      <c r="B78" s="114"/>
+      <c r="C78" s="115"/>
+      <c r="D78" s="114"/>
+      <c r="E78" s="114"/>
       <c r="F78" s="32" t="s">
         <v>253</v>
       </c>
@@ -7827,7 +7827,7 @@
       <c r="M78" s="36"/>
       <c r="N78" s="66"/>
     </row>
-    <row r="79" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A79" s="62" t="s">
         <v>254</v>
       </c>
@@ -7859,20 +7859,20 @@
       <c r="M79" s="36"/>
       <c r="N79" s="66"/>
     </row>
-    <row r="80" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="131" t="s">
+    <row r="80" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="114" t="s">
         <v>257</v>
       </c>
-      <c r="B80" s="131" t="s">
+      <c r="B80" s="114" t="s">
         <v>240</v>
       </c>
-      <c r="C80" s="133">
+      <c r="C80" s="115">
         <v>42599</v>
       </c>
-      <c r="D80" s="131" t="s">
+      <c r="D80" s="114" t="s">
         <v>241</v>
       </c>
-      <c r="E80" s="131" t="s">
+      <c r="E80" s="114" t="s">
         <v>258</v>
       </c>
       <c r="F80" s="32" t="s">
@@ -7891,12 +7891,12 @@
       <c r="M80" s="36"/>
       <c r="N80" s="66"/>
     </row>
-    <row r="81" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="131"/>
-      <c r="B81" s="131"/>
-      <c r="C81" s="133"/>
-      <c r="D81" s="131"/>
-      <c r="E81" s="131"/>
+    <row r="81" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="114"/>
+      <c r="B81" s="114"/>
+      <c r="C81" s="115"/>
+      <c r="D81" s="114"/>
+      <c r="E81" s="114"/>
       <c r="F81" s="32" t="s">
         <v>260</v>
       </c>
@@ -7915,7 +7915,7 @@
       <c r="M81" s="36"/>
       <c r="N81" s="66"/>
     </row>
-    <row r="82" spans="1:14" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="32" t="s">
         <v>261</v>
       </c>
@@ -7949,17 +7949,17 @@
       <c r="M82" s="69"/>
       <c r="N82" s="66"/>
     </row>
-    <row r="83" spans="1:14" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="131" t="s">
+    <row r="83" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="114" t="s">
         <v>266</v>
       </c>
-      <c r="B83" s="131" t="s">
+      <c r="B83" s="114" t="s">
         <v>267</v>
       </c>
-      <c r="C83" s="133">
+      <c r="C83" s="115">
         <v>42599</v>
       </c>
-      <c r="D83" s="131" t="s">
+      <c r="D83" s="114" t="s">
         <v>263</v>
       </c>
       <c r="E83" s="32" t="s">
@@ -7968,68 +7968,68 @@
       <c r="F83" s="32" t="s">
         <v>269</v>
       </c>
-      <c r="G83" s="136"/>
-      <c r="H83" s="136" t="s">
-        <v>47</v>
-      </c>
-      <c r="I83" s="136"/>
+      <c r="G83" s="121"/>
+      <c r="H83" s="121" t="s">
+        <v>47</v>
+      </c>
+      <c r="I83" s="121"/>
       <c r="J83" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="K83" s="137" t="s">
+      <c r="K83" s="122" t="s">
         <v>105</v>
       </c>
       <c r="L83" s="38"/>
       <c r="M83" s="36"/>
       <c r="N83" s="66"/>
     </row>
-    <row r="84" spans="1:14" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="131"/>
-      <c r="B84" s="131"/>
-      <c r="C84" s="133"/>
-      <c r="D84" s="131"/>
-      <c r="E84" s="138" t="s">
+    <row r="84" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="114"/>
+      <c r="B84" s="114"/>
+      <c r="C84" s="115"/>
+      <c r="D84" s="114"/>
+      <c r="E84" s="123" t="s">
         <v>270</v>
       </c>
       <c r="F84" s="56" t="s">
         <v>271</v>
       </c>
-      <c r="G84" s="136"/>
-      <c r="H84" s="136"/>
-      <c r="I84" s="136"/>
+      <c r="G84" s="121"/>
+      <c r="H84" s="121"/>
+      <c r="I84" s="121"/>
       <c r="J84" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="K84" s="137"/>
+      <c r="K84" s="122"/>
       <c r="L84" s="38"/>
       <c r="M84" s="36"/>
       <c r="N84" s="66"/>
     </row>
-    <row r="85" spans="1:14" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="131"/>
-      <c r="B85" s="131"/>
-      <c r="C85" s="133"/>
-      <c r="D85" s="131"/>
-      <c r="E85" s="138"/>
+    <row r="85" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A85" s="114"/>
+      <c r="B85" s="114"/>
+      <c r="C85" s="115"/>
+      <c r="D85" s="114"/>
+      <c r="E85" s="123"/>
       <c r="F85" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="G85" s="136"/>
-      <c r="H85" s="136"/>
-      <c r="I85" s="136"/>
+      <c r="G85" s="121"/>
+      <c r="H85" s="121"/>
+      <c r="I85" s="121"/>
       <c r="J85" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="K85" s="137"/>
+      <c r="K85" s="122"/>
       <c r="L85" s="38"/>
       <c r="M85" s="36"/>
       <c r="N85" s="66"/>
     </row>
-    <row r="86" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="131" t="s">
+    <row r="86" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="114" t="s">
         <v>273</v>
       </c>
-      <c r="B86" s="131" t="s">
+      <c r="B86" s="114" t="s">
         <v>274</v>
       </c>
       <c r="C86" s="33">
@@ -8059,9 +8059,9 @@
       <c r="M86" s="72"/>
       <c r="N86" s="66"/>
     </row>
-    <row r="87" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="131"/>
-      <c r="B87" s="131"/>
+    <row r="87" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="114"/>
+      <c r="B87" s="114"/>
       <c r="C87" s="33">
         <v>42600</v>
       </c>
@@ -8087,17 +8087,17 @@
       <c r="M87" s="36"/>
       <c r="N87" s="66"/>
     </row>
-    <row r="88" spans="1:14" ht="89.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="131" t="s">
+    <row r="88" spans="1:14" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="114" t="s">
         <v>281</v>
       </c>
-      <c r="B88" s="131" t="s">
+      <c r="B88" s="114" t="s">
         <v>267</v>
       </c>
-      <c r="C88" s="135">
+      <c r="C88" s="119">
         <v>42599</v>
       </c>
-      <c r="D88" s="131" t="s">
+      <c r="D88" s="114" t="s">
         <v>263</v>
       </c>
       <c r="E88" s="32" t="s">
@@ -8123,11 +8123,11 @@
       <c r="M88" s="36"/>
       <c r="N88" s="66"/>
     </row>
-    <row r="89" spans="1:14" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="131"/>
-      <c r="B89" s="131"/>
-      <c r="C89" s="135"/>
-      <c r="D89" s="131"/>
+    <row r="89" spans="1:14" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A89" s="114"/>
+      <c r="B89" s="114"/>
+      <c r="C89" s="119"/>
+      <c r="D89" s="114"/>
       <c r="E89" s="40" t="s">
         <v>285</v>
       </c>
@@ -8149,12 +8149,12 @@
       <c r="M89" s="36"/>
       <c r="N89" s="66"/>
     </row>
-    <row r="90" spans="1:14" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="131"/>
-      <c r="B90" s="131"/>
-      <c r="C90" s="135"/>
-      <c r="D90" s="131"/>
-      <c r="E90" s="139"/>
+    <row r="90" spans="1:14" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A90" s="114"/>
+      <c r="B90" s="114"/>
+      <c r="C90" s="119"/>
+      <c r="D90" s="114"/>
+      <c r="E90" s="124"/>
       <c r="F90" s="32" t="s">
         <v>287</v>
       </c>
@@ -8173,12 +8173,12 @@
       <c r="M90" s="36"/>
       <c r="N90" s="66"/>
     </row>
-    <row r="91" spans="1:14" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="131"/>
-      <c r="B91" s="131"/>
-      <c r="C91" s="135"/>
-      <c r="D91" s="131"/>
-      <c r="E91" s="139"/>
+    <row r="91" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A91" s="114"/>
+      <c r="B91" s="114"/>
+      <c r="C91" s="119"/>
+      <c r="D91" s="114"/>
+      <c r="E91" s="124"/>
       <c r="F91" s="32" t="s">
         <v>288</v>
       </c>
@@ -8198,7 +8198,7 @@
       <c r="N91" s="66"/>
     </row>
     <row r="92" spans="1:14" ht="68.650000000000006" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="131" t="s">
+      <c r="A92" s="114" t="s">
         <v>281</v>
       </c>
       <c r="B92" s="62" t="s">
@@ -8233,8 +8233,8 @@
         <v>293</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="131"/>
+    <row r="93" spans="1:14" ht="51" x14ac:dyDescent="0.25">
+      <c r="A93" s="114"/>
       <c r="B93" s="62" t="s">
         <v>294</v>
       </c>
@@ -8301,8 +8301,8 @@
         <v>300</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="131" t="s">
+    <row r="95" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="114" t="s">
         <v>301</v>
       </c>
       <c r="B95" s="32" t="s">
@@ -8333,8 +8333,8 @@
       <c r="M95" s="36"/>
       <c r="N95" s="66"/>
     </row>
-    <row r="96" spans="1:14" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="131"/>
+    <row r="96" spans="1:14" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="114"/>
       <c r="B96" s="32" t="s">
         <v>306</v>
       </c>
@@ -8367,8 +8367,8 @@
         <v>310</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="131" t="s">
+    <row r="97" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A97" s="114" t="s">
         <v>311</v>
       </c>
       <c r="B97" s="32" t="s">
@@ -8399,8 +8399,8 @@
       <c r="M97" s="36"/>
       <c r="N97" s="66"/>
     </row>
-    <row r="98" spans="1:14" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="131"/>
+    <row r="98" spans="1:14" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A98" s="114"/>
       <c r="B98" s="32" t="s">
         <v>316</v>
       </c>
@@ -8433,7 +8433,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A99" s="32" t="s">
         <v>320</v>
       </c>
@@ -8465,7 +8465,7 @@
       <c r="M99" s="36"/>
       <c r="N99" s="66"/>
     </row>
-    <row r="100" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A100" s="32" t="s">
         <v>321</v>
       </c>
@@ -8497,7 +8497,7 @@
       <c r="M100" s="36"/>
       <c r="N100" s="66"/>
     </row>
-    <row r="101" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A101" s="32" t="s">
         <v>322</v>
       </c>
@@ -8529,7 +8529,7 @@
       <c r="M101" s="36"/>
       <c r="N101" s="66"/>
     </row>
-    <row r="102" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A102" s="32" t="s">
         <v>326</v>
       </c>
@@ -8561,17 +8561,17 @@
       <c r="M102" s="36"/>
       <c r="N102" s="66"/>
     </row>
-    <row r="103" spans="1:14" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="131" t="s">
+    <row r="103" spans="1:14" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A103" s="114" t="s">
         <v>327</v>
       </c>
-      <c r="B103" s="131" t="s">
+      <c r="B103" s="114" t="s">
         <v>312</v>
       </c>
-      <c r="C103" s="135">
+      <c r="C103" s="119">
         <v>42600</v>
       </c>
-      <c r="D103" s="131" t="s">
+      <c r="D103" s="114" t="s">
         <v>328</v>
       </c>
       <c r="E103" s="32" t="s">
@@ -8595,11 +8595,11 @@
       <c r="M103" s="36"/>
       <c r="N103" s="66"/>
     </row>
-    <row r="104" spans="1:14" ht="47.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="131"/>
-      <c r="B104" s="131"/>
-      <c r="C104" s="135"/>
-      <c r="D104" s="131"/>
+    <row r="104" spans="1:14" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A104" s="114"/>
+      <c r="B104" s="114"/>
+      <c r="C104" s="119"/>
+      <c r="D104" s="114"/>
       <c r="E104" s="32" t="s">
         <v>331</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="52" t="s">
         <v>339</v>
       </c>
@@ -8675,11 +8675,11 @@
       <c r="E106" s="32" t="s">
         <v>342</v>
       </c>
-      <c r="F106" s="131" t="s">
+      <c r="F106" s="114" t="s">
         <v>343</v>
       </c>
       <c r="G106" s="26"/>
-      <c r="H106" s="140" t="s">
+      <c r="H106" s="120" t="s">
         <v>47</v>
       </c>
       <c r="I106" s="27"/>
@@ -8691,11 +8691,11 @@
       </c>
       <c r="L106" s="104"/>
       <c r="M106" s="36"/>
-      <c r="N106" s="134" t="s">
+      <c r="N106" s="113" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A107" s="52" t="s">
         <v>345</v>
       </c>
@@ -8711,9 +8711,9 @@
       <c r="E107" s="32" t="s">
         <v>342</v>
       </c>
-      <c r="F107" s="131"/>
+      <c r="F107" s="114"/>
       <c r="G107" s="26"/>
-      <c r="H107" s="140"/>
+      <c r="H107" s="120"/>
       <c r="I107" s="27"/>
       <c r="J107" s="28" t="s">
         <v>48</v>
@@ -8723,9 +8723,9 @@
       </c>
       <c r="L107" s="104"/>
       <c r="M107" s="36"/>
-      <c r="N107" s="134"/>
-    </row>
-    <row r="108" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N107" s="113"/>
+    </row>
+    <row r="108" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A108" s="52" t="s">
         <v>346</v>
       </c>
@@ -8741,9 +8741,9 @@
       <c r="E108" s="32" t="s">
         <v>348</v>
       </c>
-      <c r="F108" s="131"/>
+      <c r="F108" s="114"/>
       <c r="G108" s="26"/>
-      <c r="H108" s="140"/>
+      <c r="H108" s="120"/>
       <c r="I108" s="27"/>
       <c r="J108" s="28" t="s">
         <v>48</v>
@@ -8753,9 +8753,9 @@
       </c>
       <c r="L108" s="104"/>
       <c r="M108" s="36"/>
-      <c r="N108" s="134"/>
-    </row>
-    <row r="109" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N108" s="113"/>
+    </row>
+    <row r="109" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A109" s="52" t="s">
         <v>349</v>
       </c>
@@ -8823,8 +8823,8 @@
         <v>355</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="131" t="s">
+    <row r="111" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A111" s="114" t="s">
         <v>356</v>
       </c>
       <c r="B111" s="32" t="s">
@@ -8859,18 +8859,18 @@
         <v>361</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A112" s="131"/>
-      <c r="B112" s="131" t="s">
+    <row r="112" spans="1:14" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A112" s="114"/>
+      <c r="B112" s="114" t="s">
         <v>362</v>
       </c>
-      <c r="C112" s="133">
+      <c r="C112" s="115">
         <v>42601</v>
       </c>
-      <c r="D112" s="130" t="s">
+      <c r="D112" s="116" t="s">
         <v>363</v>
       </c>
-      <c r="E112" s="131" t="s">
+      <c r="E112" s="114" t="s">
         <v>364</v>
       </c>
       <c r="F112" s="32" t="s">
@@ -8889,12 +8889,12 @@
       <c r="M112" s="36"/>
       <c r="N112" s="66"/>
     </row>
-    <row r="113" spans="1:14" ht="51" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A113" s="131"/>
-      <c r="B113" s="131"/>
-      <c r="C113" s="133"/>
-      <c r="D113" s="130"/>
-      <c r="E113" s="131"/>
+    <row r="113" spans="1:14" ht="51" x14ac:dyDescent="0.25">
+      <c r="A113" s="114"/>
+      <c r="B113" s="114"/>
+      <c r="C113" s="115"/>
+      <c r="D113" s="116"/>
+      <c r="E113" s="114"/>
       <c r="F113" s="32" t="s">
         <v>365</v>
       </c>
@@ -8913,11 +8913,11 @@
       <c r="M113" s="36"/>
       <c r="N113" s="66"/>
     </row>
-    <row r="114" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="131"/>
-      <c r="B114" s="131"/>
-      <c r="C114" s="133"/>
-      <c r="D114" s="130"/>
+    <row r="114" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A114" s="114"/>
+      <c r="B114" s="114"/>
+      <c r="C114" s="115"/>
+      <c r="D114" s="116"/>
       <c r="E114" s="32" t="s">
         <v>366</v>
       </c>
@@ -8939,8 +8939,8 @@
       <c r="M114" s="36"/>
       <c r="N114" s="66"/>
     </row>
-    <row r="115" spans="1:14" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A115" s="131" t="s">
+    <row r="115" spans="1:14" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A115" s="114" t="s">
         <v>368</v>
       </c>
       <c r="B115" s="32" t="s">
@@ -8973,8 +8973,8 @@
       <c r="M115" s="36"/>
       <c r="N115" s="66"/>
     </row>
-    <row r="116" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A116" s="131"/>
+    <row r="116" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A116" s="114"/>
       <c r="B116" s="32" t="s">
         <v>371</v>
       </c>
@@ -9005,8 +9005,8 @@
       <c r="M116" s="36"/>
       <c r="N116" s="66"/>
     </row>
-    <row r="117" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="131"/>
+    <row r="117" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A117" s="114"/>
       <c r="B117" s="32" t="s">
         <v>375</v>
       </c>
@@ -9035,7 +9035,7 @@
       <c r="M117" s="36"/>
       <c r="N117" s="66"/>
     </row>
-    <row r="118" spans="1:14" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A118" s="32" t="s">
         <v>379</v>
       </c>
@@ -9065,7 +9065,7 @@
       <c r="M118" s="36"/>
       <c r="N118" s="66"/>
     </row>
-    <row r="119" spans="1:14" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A119" s="32" t="s">
         <v>382</v>
       </c>
@@ -9095,7 +9095,7 @@
       <c r="M119" s="36"/>
       <c r="N119" s="66"/>
     </row>
-    <row r="120" spans="1:14" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A120" s="32" t="s">
         <v>386</v>
       </c>
@@ -9126,16 +9126,16 @@
       <c r="N120" s="78"/>
     </row>
     <row r="121" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A121" s="143"/>
-      <c r="B121" s="143"/>
-      <c r="C121" s="143"/>
-      <c r="D121" s="143"/>
-      <c r="E121" s="143"/>
-      <c r="F121" s="143"/>
-      <c r="G121" s="143"/>
-      <c r="H121" s="143"/>
-      <c r="I121" s="143"/>
-      <c r="J121" s="143"/>
+      <c r="A121" s="117"/>
+      <c r="B121" s="117"/>
+      <c r="C121" s="117"/>
+      <c r="D121" s="117"/>
+      <c r="E121" s="117"/>
+      <c r="F121" s="117"/>
+      <c r="G121" s="117"/>
+      <c r="H121" s="117"/>
+      <c r="I121" s="117"/>
+      <c r="J121" s="117"/>
       <c r="K121" s="79"/>
       <c r="L121" s="31"/>
       <c r="M121" s="31"/>
@@ -9193,10 +9193,10 @@
       <c r="M124" s="4"/>
     </row>
     <row r="125" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="141" t="s">
+      <c r="A125" s="111" t="s">
         <v>393</v>
       </c>
-      <c r="B125" s="144"/>
+      <c r="B125" s="118"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
@@ -9210,8 +9210,8 @@
       <c r="M125" s="4"/>
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A126" s="141"/>
-      <c r="B126" s="144"/>
+      <c r="A126" s="111"/>
+      <c r="B126" s="118"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
@@ -9225,8 +9225,8 @@
       <c r="M126" s="4"/>
     </row>
     <row r="127" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A127" s="141"/>
-      <c r="B127" s="144"/>
+      <c r="A127" s="111"/>
+      <c r="B127" s="118"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
@@ -9240,10 +9240,10 @@
       <c r="M127" s="4"/>
     </row>
     <row r="128" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="141" t="s">
+      <c r="A128" s="111" t="s">
         <v>394</v>
       </c>
-      <c r="B128" s="142"/>
+      <c r="B128" s="112"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
@@ -9257,8 +9257,8 @@
       <c r="M128" s="4"/>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A129" s="141"/>
-      <c r="B129" s="142"/>
+      <c r="A129" s="111"/>
+      <c r="B129" s="112"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
@@ -9272,8 +9272,8 @@
       <c r="M129" s="4"/>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A130" s="141"/>
-      <c r="B130" s="142"/>
+      <c r="A130" s="111"/>
+      <c r="B130" s="112"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
@@ -9287,10 +9287,10 @@
       <c r="M130" s="4"/>
     </row>
     <row r="131" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="141" t="s">
+      <c r="A131" s="111" t="s">
         <v>395</v>
       </c>
-      <c r="B131" s="142"/>
+      <c r="B131" s="112"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
@@ -9304,8 +9304,8 @@
       <c r="M131" s="4"/>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A132" s="141"/>
-      <c r="B132" s="142"/>
+      <c r="A132" s="111"/>
+      <c r="B132" s="112"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -9319,8 +9319,8 @@
       <c r="M132" s="4"/>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A133" s="141"/>
-      <c r="B133" s="142"/>
+      <c r="A133" s="111"/>
+      <c r="B133" s="112"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
@@ -9335,92 +9335,15 @@
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="A128:A130"/>
-    <mergeCell ref="B128:B130"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="B131:B133"/>
-    <mergeCell ref="N106:N108"/>
-    <mergeCell ref="A111:A114"/>
-    <mergeCell ref="B112:B114"/>
-    <mergeCell ref="C112:C114"/>
-    <mergeCell ref="D112:D114"/>
-    <mergeCell ref="E112:E113"/>
-    <mergeCell ref="A115:A117"/>
-    <mergeCell ref="A121:J121"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A103:A104"/>
-    <mergeCell ref="B103:B104"/>
-    <mergeCell ref="C103:C104"/>
-    <mergeCell ref="D103:D104"/>
-    <mergeCell ref="F106:F108"/>
-    <mergeCell ref="H106:H108"/>
-    <mergeCell ref="G83:G85"/>
-    <mergeCell ref="H83:H85"/>
-    <mergeCell ref="I83:I85"/>
-    <mergeCell ref="K83:K85"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="A88:A91"/>
-    <mergeCell ref="B88:B91"/>
-    <mergeCell ref="C88:C91"/>
-    <mergeCell ref="D88:D91"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="D80:D81"/>
-    <mergeCell ref="E80:E81"/>
-    <mergeCell ref="A83:A85"/>
-    <mergeCell ref="B83:B85"/>
-    <mergeCell ref="C83:C85"/>
-    <mergeCell ref="D83:D85"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="N63:N64"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="C67:C69"/>
-    <mergeCell ref="D67:D69"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="A22:J22"/>
-    <mergeCell ref="A50:A57"/>
-    <mergeCell ref="B50:B57"/>
-    <mergeCell ref="D50:D57"/>
-    <mergeCell ref="J50:J55"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="C58:C60"/>
-    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="B1:E6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A8:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="A16:B16"/>
@@ -9436,15 +9359,92 @@
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="G19:I19"/>
     <mergeCell ref="J19:J20"/>
-    <mergeCell ref="A1:A6"/>
-    <mergeCell ref="B1:E6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A8:F9"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M19:M20"/>
+    <mergeCell ref="A22:J22"/>
+    <mergeCell ref="A50:A57"/>
+    <mergeCell ref="B50:B57"/>
+    <mergeCell ref="D50:D57"/>
+    <mergeCell ref="J50:J55"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="C58:C60"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="N63:N64"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="C67:C69"/>
+    <mergeCell ref="D67:D69"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="A80:A81"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="C80:C81"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="A83:A85"/>
+    <mergeCell ref="B83:B85"/>
+    <mergeCell ref="C83:C85"/>
+    <mergeCell ref="D83:D85"/>
+    <mergeCell ref="G83:G85"/>
+    <mergeCell ref="H83:H85"/>
+    <mergeCell ref="I83:I85"/>
+    <mergeCell ref="K83:K85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="A86:A87"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="A88:A91"/>
+    <mergeCell ref="B88:B91"/>
+    <mergeCell ref="C88:C91"/>
+    <mergeCell ref="D88:D91"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="A92:A93"/>
+    <mergeCell ref="A95:A96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="A103:A104"/>
+    <mergeCell ref="B103:B104"/>
+    <mergeCell ref="C103:C104"/>
+    <mergeCell ref="D103:D104"/>
+    <mergeCell ref="F106:F108"/>
+    <mergeCell ref="H106:H108"/>
+    <mergeCell ref="A128:A130"/>
+    <mergeCell ref="B128:B130"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="B131:B133"/>
+    <mergeCell ref="N106:N108"/>
+    <mergeCell ref="A111:A114"/>
+    <mergeCell ref="B112:B114"/>
+    <mergeCell ref="C112:C114"/>
+    <mergeCell ref="D112:D114"/>
+    <mergeCell ref="E112:E113"/>
+    <mergeCell ref="A115:A117"/>
+    <mergeCell ref="A121:J121"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="B125:B127"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -9457,9 +9457,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK61"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="A16" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A7" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M48" activeCellId="1" sqref="M49 M48"/>
+      <selection pane="topRight" activeCell="G20" sqref="A20:XFD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9481,13 +9481,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111"/>
-      <c r="B1" s="112" t="s">
+      <c r="A1" s="139"/>
+      <c r="B1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -9498,11 +9498,11 @@
       <c r="M1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="111"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="A2" s="139"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
@@ -9515,11 +9515,11 @@
       <c r="M2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="111"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
+      <c r="A3" s="139"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
       <c r="F3" s="6" t="s">
         <v>2</v>
       </c>
@@ -9532,11 +9532,11 @@
       <c r="M3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
       <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
@@ -9549,11 +9549,11 @@
       <c r="M4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="111"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
+      <c r="A5" s="139"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140"/>
       <c r="F5" s="6"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -9564,11 +9564,11 @@
       <c r="M5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="111"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
+      <c r="A6" s="139"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
       <c r="F6" s="7"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -9583,14 +9583,14 @@
         <v>4</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113" t="s">
+      <c r="D7" s="141"/>
+      <c r="E7" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="113"/>
+      <c r="F7" s="141"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7"/>
@@ -9600,12 +9600,12 @@
       <c r="M7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8"/>
@@ -9615,12 +9615,12 @@
       <c r="M8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="114"/>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
+      <c r="A9" s="142"/>
+      <c r="B9" s="142"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9"/>
@@ -9630,14 +9630,14 @@
       <c r="M9"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="115" t="s">
+      <c r="A10" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="115"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
+      <c r="B10" s="143"/>
+      <c r="C10" s="143"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="143"/>
+      <c r="F10" s="143"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10"/>
@@ -9647,14 +9647,14 @@
       <c r="M10"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="116"/>
-      <c r="C11" s="116"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
+      <c r="B11" s="144"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="144"/>
+      <c r="F11" s="144"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="10" t="s">
@@ -9666,14 +9666,14 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
+      <c r="B12" s="144"/>
+      <c r="C12" s="144"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="144"/>
+      <c r="F12" s="144"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="11" t="s">
@@ -9685,14 +9685,14 @@
       <c r="M12"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="144"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="12" t="s">
@@ -9704,10 +9704,10 @@
       <c r="M13"/>
     </row>
     <row r="14" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="117"/>
+      <c r="B14" s="129"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
@@ -9723,10 +9723,10 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="118"/>
+      <c r="B15" s="130"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
@@ -9742,10 +9742,10 @@
       <c r="M15"/>
     </row>
     <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="119" t="s">
+      <c r="A16" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="119"/>
+      <c r="B16" s="131"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
@@ -9759,83 +9759,83 @@
       <c r="M16"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="120" t="s">
+      <c r="A17" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="121"/>
-      <c r="F17" s="121"/>
-      <c r="G17" s="121"/>
-      <c r="H17" s="121"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="121"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="133"/>
+      <c r="I17" s="133"/>
+      <c r="J17" s="133"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="122"/>
-      <c r="C18" s="145"/>
-      <c r="D18" s="145"/>
-      <c r="E18" s="145"/>
-      <c r="F18" s="145"/>
-      <c r="G18" s="145"/>
-      <c r="H18" s="145"/>
-      <c r="I18" s="145"/>
-      <c r="J18" s="145"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="148"/>
+      <c r="D18" s="148"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
+      <c r="G18" s="148"/>
+      <c r="H18" s="148"/>
+      <c r="I18" s="148"/>
+      <c r="J18" s="148"/>
       <c r="K18" s="20"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="124" t="s">
+      <c r="A19" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="125" t="s">
+      <c r="B19" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="125" t="s">
+      <c r="C19" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="124" t="s">
+      <c r="D19" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="124" t="s">
+      <c r="E19" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="124" t="s">
+      <c r="F19" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="126" t="s">
+      <c r="G19" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="126"/>
-      <c r="I19" s="126"/>
-      <c r="J19" s="124" t="s">
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="127" t="s">
+      <c r="K19" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="128" t="s">
+      <c r="L19" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="M19" s="128" t="s">
+      <c r="M19" s="126" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="124"/>
-      <c r="B20" s="125"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="124"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="124"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="136"/>
       <c r="G20" s="22" t="s">
         <v>32</v>
       </c>
@@ -9845,10 +9845,10 @@
       <c r="I20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="124"/>
-      <c r="K20" s="127"/>
-      <c r="L20" s="128"/>
-      <c r="M20" s="128"/>
+      <c r="J20" s="136"/>
+      <c r="K20" s="125"/>
+      <c r="L20" s="126"/>
+      <c r="M20" s="126"/>
     </row>
     <row r="21" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
@@ -9878,33 +9878,33 @@
       <c r="M21"/>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="147" t="s">
         <v>396</v>
       </c>
-      <c r="B22" s="146"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
-      <c r="H22" s="146"/>
-      <c r="I22" s="146"/>
-      <c r="J22" s="146"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="147"/>
+      <c r="D22" s="147"/>
+      <c r="E22" s="147"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="147"/>
+      <c r="H22" s="147"/>
+      <c r="I22" s="147"/>
+      <c r="J22" s="147"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="131" t="s">
+    <row r="23" spans="1:13" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="114" t="s">
         <v>397</v>
       </c>
-      <c r="B23" s="131" t="s">
+      <c r="B23" s="114" t="s">
         <v>398</v>
       </c>
-      <c r="C23" s="133">
+      <c r="C23" s="115">
         <v>42604</v>
       </c>
-      <c r="D23" s="131" t="s">
+      <c r="D23" s="114" t="s">
         <v>399</v>
       </c>
       <c r="E23" s="32" t="s">
@@ -9927,11 +9927,11 @@
         <v>402</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="131"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="133"/>
-      <c r="D24" s="131"/>
+    <row r="24" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="114"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="114"/>
       <c r="E24" s="40" t="s">
         <v>403</v>
       </c>
@@ -9952,7 +9952,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A25" s="32" t="s">
         <v>406</v>
       </c>
@@ -10051,7 +10051,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="51" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
         <v>425</v>
       </c>
@@ -10080,7 +10080,7 @@
       <c r="L28" s="37"/>
       <c r="M28" s="37"/>
     </row>
-    <row r="29" spans="1:13" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="62" t="s">
         <v>429</v>
       </c>
@@ -10109,7 +10109,7 @@
       <c r="L29" s="37"/>
       <c r="M29" s="37"/>
     </row>
-    <row r="30" spans="1:13" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="62" t="s">
         <v>434</v>
       </c>
@@ -10140,7 +10140,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>440</v>
       </c>
@@ -10169,7 +10169,7 @@
       <c r="L31" s="37"/>
       <c r="M31" s="37"/>
     </row>
-    <row r="32" spans="1:13" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>443</v>
       </c>
@@ -10202,20 +10202,20 @@
         <v>448</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="76.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="130" t="s">
+    <row r="33" spans="1:13" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="116" t="s">
         <v>449</v>
       </c>
-      <c r="B33" s="130" t="s">
+      <c r="B33" s="116" t="s">
         <v>450</v>
       </c>
-      <c r="C33" s="135">
+      <c r="C33" s="119">
         <v>37856</v>
       </c>
-      <c r="D33" s="131" t="s">
+      <c r="D33" s="114" t="s">
         <v>451</v>
       </c>
-      <c r="E33" s="130" t="s">
+      <c r="E33" s="116" t="s">
         <v>452</v>
       </c>
       <c r="F33" s="89" t="s">
@@ -10231,16 +10231,16 @@
         <v>417</v>
       </c>
       <c r="L33" s="86"/>
-      <c r="M33" s="147" t="s">
+      <c r="M33" s="146" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="130"/>
-      <c r="B34" s="130"/>
-      <c r="C34" s="135"/>
-      <c r="D34" s="131"/>
-      <c r="E34" s="130"/>
+    <row r="34" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="116"/>
+      <c r="B34" s="116"/>
+      <c r="C34" s="119"/>
+      <c r="D34" s="114"/>
+      <c r="E34" s="116"/>
       <c r="F34" s="89" t="s">
         <v>455</v>
       </c>
@@ -10254,13 +10254,13 @@
         <v>417</v>
       </c>
       <c r="L34" s="86"/>
-      <c r="M34" s="147"/>
-    </row>
-    <row r="35" spans="1:13" ht="127.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="130"/>
-      <c r="B35" s="130"/>
-      <c r="C35" s="135"/>
-      <c r="D35" s="131"/>
+      <c r="M34" s="146"/>
+    </row>
+    <row r="35" spans="1:13" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="116"/>
+      <c r="B35" s="116"/>
+      <c r="C35" s="119"/>
+      <c r="D35" s="114"/>
       <c r="E35" s="62" t="s">
         <v>456</v>
       </c>
@@ -10281,10 +10281,10 @@
         <v>458</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="130"/>
-      <c r="B36" s="130"/>
-      <c r="C36" s="135"/>
+    <row r="36" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="116"/>
+      <c r="B36" s="116"/>
+      <c r="C36" s="119"/>
       <c r="D36" s="52" t="s">
         <v>459</v>
       </c>
@@ -10308,10 +10308,10 @@
         <v>458</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="130"/>
-      <c r="B37" s="130"/>
-      <c r="C37" s="135"/>
+    <row r="37" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="116"/>
+      <c r="B37" s="116"/>
+      <c r="C37" s="119"/>
       <c r="D37" s="52" t="s">
         <v>462</v>
       </c>
@@ -10331,7 +10331,7 @@
       <c r="L37" s="37"/>
       <c r="M37" s="37"/>
     </row>
-    <row r="38" spans="1:13" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A38" s="92"/>
       <c r="B38" s="92"/>
       <c r="C38" s="93"/>
@@ -10356,20 +10356,20 @@
         <v>466</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="102" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="131" t="s">
+    <row r="39" spans="1:13" ht="102" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="114" t="s">
         <v>467</v>
       </c>
-      <c r="B39" s="131" t="s">
+      <c r="B39" s="114" t="s">
         <v>468</v>
       </c>
       <c r="C39" s="33">
         <v>37856</v>
       </c>
-      <c r="D39" s="131" t="s">
+      <c r="D39" s="114" t="s">
         <v>469</v>
       </c>
-      <c r="E39" s="131" t="s">
+      <c r="E39" s="114" t="s">
         <v>470</v>
       </c>
       <c r="F39" s="40" t="s">
@@ -10389,14 +10389,14 @@
         <v>472</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="63.75" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="131"/>
-      <c r="B40" s="131"/>
+    <row r="40" spans="1:13" ht="63.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="114"/>
+      <c r="B40" s="114"/>
       <c r="C40" s="33">
         <v>37856</v>
       </c>
-      <c r="D40" s="131"/>
-      <c r="E40" s="131"/>
+      <c r="D40" s="114"/>
+      <c r="E40" s="114"/>
       <c r="F40" s="40" t="s">
         <v>473</v>
       </c>
@@ -10414,7 +10414,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A41" s="91" t="s">
         <v>474</v>
       </c>
@@ -10443,7 +10443,7 @@
       <c r="L41" s="37"/>
       <c r="M41" s="37"/>
     </row>
-    <row r="42" spans="1:13" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A42" s="62" t="s">
         <v>479</v>
       </c>
@@ -10472,7 +10472,7 @@
       <c r="L42" s="37"/>
       <c r="M42" s="37"/>
     </row>
-    <row r="43" spans="1:13" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A43" s="62" t="s">
         <v>484</v>
       </c>
@@ -10534,11 +10534,11 @@
         <v>494</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="38.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="130" t="s">
+    <row r="45" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="116" t="s">
         <v>495</v>
       </c>
-      <c r="B45" s="131" t="s">
+      <c r="B45" s="114" t="s">
         <v>496</v>
       </c>
       <c r="C45" s="33"/>
@@ -10566,8 +10566,8 @@
       </c>
     </row>
     <row r="46" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A46" s="130"/>
-      <c r="B46" s="131"/>
+      <c r="A46" s="116"/>
+      <c r="B46" s="114"/>
       <c r="C46" s="33"/>
       <c r="D46" s="32" t="s">
         <v>501</v>
@@ -10592,9 +10592,9 @@
         <v>504</v>
       </c>
     </row>
-    <row r="47" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="130"/>
-      <c r="B47" s="131"/>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="116"/>
+      <c r="B47" s="114"/>
       <c r="C47" s="33"/>
       <c r="D47" s="32" t="s">
         <v>505</v>
@@ -10616,8 +10616,8 @@
       <c r="M47" s="37"/>
     </row>
     <row r="48" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="130"/>
-      <c r="B48" s="131"/>
+      <c r="A48" s="116"/>
+      <c r="B48" s="114"/>
       <c r="C48" s="33"/>
       <c r="D48" s="32" t="s">
         <v>508</v>
@@ -10643,16 +10643,16 @@
       </c>
     </row>
     <row r="49" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="148"/>
-      <c r="B49" s="148"/>
-      <c r="C49" s="148"/>
-      <c r="D49" s="148"/>
-      <c r="E49" s="148"/>
-      <c r="F49" s="148"/>
-      <c r="G49" s="148"/>
-      <c r="H49" s="148"/>
-      <c r="I49" s="148"/>
-      <c r="J49" s="148"/>
+      <c r="A49" s="145"/>
+      <c r="B49" s="145"/>
+      <c r="C49" s="145"/>
+      <c r="D49" s="145"/>
+      <c r="E49" s="145"/>
+      <c r="F49" s="145"/>
+      <c r="G49" s="145"/>
+      <c r="H49" s="145"/>
+      <c r="I49" s="145"/>
+      <c r="J49" s="145"/>
       <c r="K49" s="94"/>
       <c r="L49" s="94"/>
       <c r="M49" s="54"/>
@@ -10697,10 +10697,10 @@
       <c r="M52" s="37"/>
     </row>
     <row r="53" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="141" t="s">
+      <c r="A53" s="111" t="s">
         <v>393</v>
       </c>
-      <c r="B53" s="144"/>
+      <c r="B53" s="118"/>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
       <c r="K53" s="37"/>
@@ -10708,8 +10708,8 @@
       <c r="M53" s="37"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" s="141"/>
-      <c r="B54" s="144"/>
+      <c r="A54" s="111"/>
+      <c r="B54" s="118"/>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
       <c r="K54" s="37"/>
@@ -10717,8 +10717,8 @@
       <c r="M54" s="37"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A55" s="141"/>
-      <c r="B55" s="144"/>
+      <c r="A55" s="111"/>
+      <c r="B55" s="118"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
       <c r="K55" s="37"/>
@@ -10726,10 +10726,10 @@
       <c r="M55" s="37"/>
     </row>
     <row r="56" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="141" t="s">
+      <c r="A56" s="111" t="s">
         <v>394</v>
       </c>
-      <c r="B56" s="142"/>
+      <c r="B56" s="112"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
       <c r="K56" s="37"/>
@@ -10737,8 +10737,8 @@
       <c r="M56" s="37"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A57" s="141"/>
-      <c r="B57" s="142"/>
+      <c r="A57" s="111"/>
+      <c r="B57" s="112"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
       <c r="K57" s="37"/>
@@ -10746,8 +10746,8 @@
       <c r="M57" s="37"/>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A58" s="141"/>
-      <c r="B58" s="142"/>
+      <c r="A58" s="111"/>
+      <c r="B58" s="112"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
       <c r="K58" s="37"/>
@@ -10755,10 +10755,10 @@
       <c r="M58" s="37"/>
     </row>
     <row r="59" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="141" t="s">
+      <c r="A59" s="111" t="s">
         <v>395</v>
       </c>
-      <c r="B59" s="142"/>
+      <c r="B59" s="112"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
       <c r="K59" s="37"/>
@@ -10766,8 +10766,8 @@
       <c r="M59" s="37"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A60" s="141"/>
-      <c r="B60" s="142"/>
+      <c r="A60" s="111"/>
+      <c r="B60" s="112"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
       <c r="K60" s="37"/>
@@ -10775,8 +10775,8 @@
       <c r="M60" s="37"/>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A61" s="141"/>
-      <c r="B61" s="142"/>
+      <c r="A61" s="111"/>
+      <c r="B61" s="112"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
       <c r="K61" s="37"/>
@@ -10785,25 +10785,22 @@
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="B59:B61"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A49:J49"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="M33:M34"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="C33:C37"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="B1:E6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A8:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:J18"/>
     <mergeCell ref="M19:M20"/>
     <mergeCell ref="A22:J22"/>
     <mergeCell ref="A23:A24"/>
@@ -10820,22 +10817,25 @@
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:J18"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A1:A6"/>
-    <mergeCell ref="B1:E6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A8:F9"/>
+    <mergeCell ref="M33:M34"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="C33:C37"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="B59:B61"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B45:B48"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="B53:B55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
@@ -10847,8 +10847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView windowProtection="1" topLeftCell="C16" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView windowProtection="1" topLeftCell="C13" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10870,13 +10870,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111"/>
-      <c r="B1" s="112" t="s">
+      <c r="A1" s="139"/>
+      <c r="B1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -10887,11 +10887,11 @@
       <c r="M1" s="4"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="111"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="A2" s="139"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
@@ -10904,11 +10904,11 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="111"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
+      <c r="A3" s="139"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
       <c r="F3" s="6" t="s">
         <v>2</v>
       </c>
@@ -10921,11 +10921,11 @@
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
       <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
@@ -10938,11 +10938,11 @@
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="111"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
+      <c r="A5" s="139"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140"/>
       <c r="F5" s="6"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -10953,11 +10953,11 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="111"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
+      <c r="A6" s="139"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
       <c r="F6" s="7"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -10972,14 +10972,14 @@
         <v>4</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113" t="s">
+      <c r="D7" s="141"/>
+      <c r="E7" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="113"/>
+      <c r="F7" s="141"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="4"/>
@@ -10989,12 +10989,12 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="4"/>
@@ -11004,12 +11004,12 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="114"/>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
+      <c r="A9" s="142"/>
+      <c r="B9" s="142"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="4"/>
@@ -11019,14 +11019,14 @@
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="115" t="s">
+      <c r="A10" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="115"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
+      <c r="B10" s="143"/>
+      <c r="C10" s="143"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="143"/>
+      <c r="F10" s="143"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="4"/>
@@ -11036,14 +11036,14 @@
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="116"/>
-      <c r="C11" s="116"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
+      <c r="B11" s="144"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="144"/>
+      <c r="F11" s="144"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="4"/>
@@ -11053,14 +11053,14 @@
       <c r="M11" s="4"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
+      <c r="B12" s="144"/>
+      <c r="C12" s="144"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="144"/>
+      <c r="F12" s="144"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="4"/>
@@ -11070,14 +11070,14 @@
       <c r="M12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="144"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="4"/>
@@ -11087,10 +11087,10 @@
       <c r="M13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="117"/>
+      <c r="B14" s="129"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -11104,10 +11104,10 @@
       <c r="M14" s="4"/>
     </row>
     <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="118"/>
+      <c r="B15" s="130"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -11121,10 +11121,10 @@
       <c r="M15" s="4"/>
     </row>
     <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="119" t="s">
+      <c r="A16" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="119"/>
+      <c r="B16" s="131"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -11138,83 +11138,83 @@
       <c r="M16" s="4"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="120" t="s">
+      <c r="A17" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="121"/>
-      <c r="F17" s="121"/>
-      <c r="G17" s="121"/>
-      <c r="H17" s="121"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="121"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="133"/>
+      <c r="I17" s="133"/>
+      <c r="J17" s="133"/>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="122"/>
-      <c r="C18" s="145"/>
-      <c r="D18" s="145"/>
-      <c r="E18" s="145"/>
-      <c r="F18" s="145"/>
-      <c r="G18" s="145"/>
-      <c r="H18" s="145"/>
-      <c r="I18" s="145"/>
-      <c r="J18" s="145"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="148"/>
+      <c r="D18" s="148"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
+      <c r="G18" s="148"/>
+      <c r="H18" s="148"/>
+      <c r="I18" s="148"/>
+      <c r="J18" s="148"/>
       <c r="K18" s="20"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="124" t="s">
+      <c r="A19" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="125" t="s">
+      <c r="B19" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="125" t="s">
+      <c r="C19" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="124" t="s">
+      <c r="D19" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="124" t="s">
+      <c r="E19" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="124" t="s">
+      <c r="F19" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="126" t="s">
+      <c r="G19" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="126"/>
-      <c r="I19" s="126"/>
-      <c r="J19" s="124" t="s">
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="127" t="s">
+      <c r="K19" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="128" t="s">
+      <c r="L19" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="M19" s="128" t="s">
+      <c r="M19" s="126" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="124"/>
-      <c r="B20" s="125"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="124"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="124"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="136"/>
       <c r="G20" s="22" t="s">
         <v>32</v>
       </c>
@@ -11224,10 +11224,10 @@
       <c r="I20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="124"/>
-      <c r="K20" s="127"/>
-      <c r="L20" s="128"/>
-      <c r="M20" s="128"/>
+      <c r="J20" s="136"/>
+      <c r="K20" s="125"/>
+      <c r="L20" s="126"/>
+      <c r="M20" s="126"/>
     </row>
     <row r="21" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
@@ -11257,18 +11257,18 @@
       <c r="M21" s="4"/>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="147" t="s">
         <v>396</v>
       </c>
-      <c r="B22" s="146"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
-      <c r="H22" s="146"/>
-      <c r="I22" s="146"/>
-      <c r="J22" s="146"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="147"/>
+      <c r="D22" s="147"/>
+      <c r="E22" s="147"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="147"/>
+      <c r="H22" s="147"/>
+      <c r="I22" s="147"/>
+      <c r="J22" s="147"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -11339,7 +11339,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="102" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="102" x14ac:dyDescent="0.25">
       <c r="A25" s="52" t="s">
         <v>425</v>
       </c>
@@ -11368,7 +11368,7 @@
       <c r="L25" s="4"/>
       <c r="M25" s="4"/>
     </row>
-    <row r="26" spans="1:13" ht="89.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="89.25" x14ac:dyDescent="0.25">
       <c r="A26" s="52" t="s">
         <v>515</v>
       </c>
@@ -11433,16 +11433,16 @@
       </c>
     </row>
     <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="148"/>
-      <c r="B28" s="148"/>
-      <c r="C28" s="148"/>
-      <c r="D28" s="148"/>
-      <c r="E28" s="148"/>
-      <c r="F28" s="148"/>
-      <c r="G28" s="148"/>
-      <c r="H28" s="148"/>
-      <c r="I28" s="148"/>
-      <c r="J28" s="148"/>
+      <c r="A28" s="145"/>
+      <c r="B28" s="145"/>
+      <c r="C28" s="145"/>
+      <c r="D28" s="145"/>
+      <c r="E28" s="145"/>
+      <c r="F28" s="145"/>
+      <c r="G28" s="145"/>
+      <c r="H28" s="145"/>
+      <c r="I28" s="145"/>
+      <c r="J28" s="145"/>
       <c r="K28" s="82"/>
       <c r="L28" s="82"/>
       <c r="M28" s="97"/>
@@ -11499,10 +11499,10 @@
       <c r="M31" s="4"/>
     </row>
     <row r="32" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="141" t="s">
+      <c r="A32" s="111" t="s">
         <v>393</v>
       </c>
-      <c r="B32" s="144"/>
+      <c r="B32" s="118"/>
       <c r="C32" s="4"/>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
@@ -11516,8 +11516,8 @@
       <c r="M32" s="4"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="141"/>
-      <c r="B33" s="144"/>
+      <c r="A33" s="111"/>
+      <c r="B33" s="118"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
@@ -11531,8 +11531,8 @@
       <c r="M33" s="4"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="141"/>
-      <c r="B34" s="144"/>
+      <c r="A34" s="111"/>
+      <c r="B34" s="118"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
@@ -11546,10 +11546,10 @@
       <c r="M34" s="4"/>
     </row>
     <row r="35" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="141" t="s">
+      <c r="A35" s="111" t="s">
         <v>394</v>
       </c>
-      <c r="B35" s="142"/>
+      <c r="B35" s="112"/>
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
@@ -11563,8 +11563,8 @@
       <c r="M35" s="4"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="141"/>
-      <c r="B36" s="142"/>
+      <c r="A36" s="111"/>
+      <c r="B36" s="112"/>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
@@ -11578,8 +11578,8 @@
       <c r="M36" s="4"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="141"/>
-      <c r="B37" s="142"/>
+      <c r="A37" s="111"/>
+      <c r="B37" s="112"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
@@ -11593,10 +11593,10 @@
       <c r="M37" s="4"/>
     </row>
     <row r="38" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="141" t="s">
+      <c r="A38" s="111" t="s">
         <v>395</v>
       </c>
-      <c r="B38" s="142"/>
+      <c r="B38" s="112"/>
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
@@ -11610,8 +11610,8 @@
       <c r="M38" s="4"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="141"/>
-      <c r="B39" s="142"/>
+      <c r="A39" s="111"/>
+      <c r="B39" s="112"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
@@ -11625,8 +11625,8 @@
       <c r="M39" s="4"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="141"/>
-      <c r="B40" s="142"/>
+      <c r="A40" s="111"/>
+      <c r="B40" s="112"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
@@ -11641,6 +11641,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="B1:E6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A8:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:J18"/>
     <mergeCell ref="A35:A37"/>
     <mergeCell ref="B35:B37"/>
     <mergeCell ref="A38:A40"/>
@@ -11657,25 +11676,6 @@
     <mergeCell ref="L19:L20"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:J18"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A1:A6"/>
-    <mergeCell ref="B1:E6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A8:F9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -11687,10 +11687,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK52"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" topLeftCell="A16" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+    <sheetView windowProtection="1" topLeftCell="A28" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
       <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="L31" sqref="L31"/>
+      <selection pane="topRight" activeCell="M33" sqref="M33:M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11712,13 +11712,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="111"/>
-      <c r="B1" s="112" t="s">
+      <c r="A1" s="139"/>
+      <c r="B1" s="140" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="112"/>
-      <c r="D1" s="112"/>
-      <c r="E1" s="112"/>
+      <c r="C1" s="140"/>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
       <c r="F1" s="2"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
@@ -11729,11 +11729,11 @@
       <c r="M1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="111"/>
-      <c r="B2" s="112"/>
-      <c r="C2" s="112"/>
-      <c r="D2" s="112"/>
-      <c r="E2" s="112"/>
+      <c r="A2" s="139"/>
+      <c r="B2" s="140"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
       <c r="F2" s="5" t="s">
         <v>1</v>
       </c>
@@ -11746,11 +11746,11 @@
       <c r="M2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="111"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
+      <c r="A3" s="139"/>
+      <c r="B3" s="140"/>
+      <c r="C3" s="140"/>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
       <c r="F3" s="6" t="s">
         <v>2</v>
       </c>
@@ -11763,11 +11763,11 @@
       <c r="M3"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="111"/>
-      <c r="B4" s="112"/>
-      <c r="C4" s="112"/>
-      <c r="D4" s="112"/>
-      <c r="E4" s="112"/>
+      <c r="A4" s="139"/>
+      <c r="B4" s="140"/>
+      <c r="C4" s="140"/>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
       <c r="F4" s="6" t="s">
         <v>3</v>
       </c>
@@ -11780,11 +11780,11 @@
       <c r="M4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="111"/>
-      <c r="B5" s="112"/>
-      <c r="C5" s="112"/>
-      <c r="D5" s="112"/>
-      <c r="E5" s="112"/>
+      <c r="A5" s="139"/>
+      <c r="B5" s="140"/>
+      <c r="C5" s="140"/>
+      <c r="D5" s="140"/>
+      <c r="E5" s="140"/>
       <c r="F5" s="6"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -11795,11 +11795,11 @@
       <c r="M5"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="111"/>
-      <c r="B6" s="112"/>
-      <c r="C6" s="112"/>
-      <c r="D6" s="112"/>
-      <c r="E6" s="112"/>
+      <c r="A6" s="139"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
       <c r="F6" s="7"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
@@ -11814,14 +11814,14 @@
         <v>4</v>
       </c>
       <c r="B7" s="9"/>
-      <c r="C7" s="113" t="s">
+      <c r="C7" s="141" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113" t="s">
+      <c r="D7" s="141"/>
+      <c r="E7" s="141" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="113"/>
+      <c r="F7" s="141"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7"/>
@@ -11831,12 +11831,12 @@
       <c r="M7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="114"/>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
-      <c r="D8" s="114"/>
-      <c r="E8" s="114"/>
-      <c r="F8" s="114"/>
+      <c r="A8" s="142"/>
+      <c r="B8" s="142"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="142"/>
+      <c r="E8" s="142"/>
+      <c r="F8" s="142"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8"/>
@@ -11846,12 +11846,12 @@
       <c r="M8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="114"/>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
+      <c r="A9" s="142"/>
+      <c r="B9" s="142"/>
+      <c r="C9" s="142"/>
+      <c r="D9" s="142"/>
+      <c r="E9" s="142"/>
+      <c r="F9" s="142"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9"/>
@@ -11861,14 +11861,14 @@
       <c r="M9"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="115" t="s">
+      <c r="A10" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="115"/>
-      <c r="C10" s="115"/>
-      <c r="D10" s="115"/>
-      <c r="E10" s="115"/>
-      <c r="F10" s="115"/>
+      <c r="B10" s="143"/>
+      <c r="C10" s="143"/>
+      <c r="D10" s="143"/>
+      <c r="E10" s="143"/>
+      <c r="F10" s="143"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10"/>
@@ -11878,14 +11878,14 @@
       <c r="M10"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="144" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="116"/>
-      <c r="C11" s="116"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
+      <c r="B11" s="144"/>
+      <c r="C11" s="144"/>
+      <c r="D11" s="144"/>
+      <c r="E11" s="144"/>
+      <c r="F11" s="144"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11"/>
@@ -11895,14 +11895,14 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="144" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="116"/>
-      <c r="C12" s="116"/>
-      <c r="D12" s="116"/>
-      <c r="E12" s="116"/>
-      <c r="F12" s="116"/>
+      <c r="B12" s="144"/>
+      <c r="C12" s="144"/>
+      <c r="D12" s="144"/>
+      <c r="E12" s="144"/>
+      <c r="F12" s="144"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12"/>
@@ -11912,14 +11912,14 @@
       <c r="M12"/>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="144" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="116"/>
-      <c r="C13" s="116"/>
-      <c r="D13" s="116"/>
-      <c r="E13" s="116"/>
-      <c r="F13" s="116"/>
+      <c r="B13" s="144"/>
+      <c r="C13" s="144"/>
+      <c r="D13" s="144"/>
+      <c r="E13" s="144"/>
+      <c r="F13" s="144"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13"/>
@@ -11929,10 +11929,10 @@
       <c r="M13"/>
     </row>
     <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="117" t="s">
+      <c r="A14" s="129" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="117"/>
+      <c r="B14" s="129"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
@@ -11946,10 +11946,10 @@
       <c r="M14"/>
     </row>
     <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="118" t="s">
+      <c r="A15" s="130" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="118"/>
+      <c r="B15" s="130"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
@@ -11963,10 +11963,10 @@
       <c r="M15"/>
     </row>
     <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="119" t="s">
+      <c r="A16" s="131" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="119"/>
+      <c r="B16" s="131"/>
       <c r="C16"/>
       <c r="D16"/>
       <c r="E16"/>
@@ -11980,83 +11980,83 @@
       <c r="M16"/>
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="120" t="s">
+      <c r="A17" s="132" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="120"/>
-      <c r="C17" s="121"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="121"/>
-      <c r="F17" s="121"/>
-      <c r="G17" s="121"/>
-      <c r="H17" s="121"/>
-      <c r="I17" s="121"/>
-      <c r="J17" s="121"/>
+      <c r="B17" s="132"/>
+      <c r="C17" s="133"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="133"/>
+      <c r="F17" s="133"/>
+      <c r="G17" s="133"/>
+      <c r="H17" s="133"/>
+      <c r="I17" s="133"/>
+      <c r="J17" s="133"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="122" t="s">
+      <c r="A18" s="134" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="122"/>
-      <c r="C18" s="145"/>
-      <c r="D18" s="145"/>
-      <c r="E18" s="145"/>
-      <c r="F18" s="145"/>
-      <c r="G18" s="145"/>
-      <c r="H18" s="145"/>
-      <c r="I18" s="145"/>
-      <c r="J18" s="145"/>
+      <c r="B18" s="134"/>
+      <c r="C18" s="148"/>
+      <c r="D18" s="148"/>
+      <c r="E18" s="148"/>
+      <c r="F18" s="148"/>
+      <c r="G18" s="148"/>
+      <c r="H18" s="148"/>
+      <c r="I18" s="148"/>
+      <c r="J18" s="148"/>
       <c r="K18" s="20"/>
       <c r="L18" s="21"/>
       <c r="M18" s="21"/>
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="124" t="s">
+      <c r="A19" s="136" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="125" t="s">
+      <c r="B19" s="137" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="125" t="s">
+      <c r="C19" s="137" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="124" t="s">
+      <c r="D19" s="136" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="124" t="s">
+      <c r="E19" s="136" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="124" t="s">
+      <c r="F19" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="126" t="s">
+      <c r="G19" s="138" t="s">
         <v>27</v>
       </c>
-      <c r="H19" s="126"/>
-      <c r="I19" s="126"/>
-      <c r="J19" s="124" t="s">
+      <c r="H19" s="138"/>
+      <c r="I19" s="138"/>
+      <c r="J19" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="K19" s="127" t="s">
+      <c r="K19" s="125" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="128" t="s">
+      <c r="L19" s="126" t="s">
         <v>30</v>
       </c>
-      <c r="M19" s="128" t="s">
+      <c r="M19" s="126" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="124"/>
-      <c r="B20" s="125"/>
-      <c r="C20" s="125"/>
-      <c r="D20" s="124"/>
-      <c r="E20" s="124"/>
-      <c r="F20" s="124"/>
+      <c r="A20" s="136"/>
+      <c r="B20" s="137"/>
+      <c r="C20" s="137"/>
+      <c r="D20" s="136"/>
+      <c r="E20" s="136"/>
+      <c r="F20" s="136"/>
       <c r="G20" s="22" t="s">
         <v>32</v>
       </c>
@@ -12066,10 +12066,10 @@
       <c r="I20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="J20" s="124"/>
-      <c r="K20" s="127"/>
-      <c r="L20" s="128"/>
-      <c r="M20" s="128"/>
+      <c r="J20" s="136"/>
+      <c r="K20" s="125"/>
+      <c r="L20" s="126"/>
+      <c r="M20" s="126"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
@@ -12099,33 +12099,33 @@
       <c r="M21"/>
     </row>
     <row r="22" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="146" t="s">
+      <c r="A22" s="147" t="s">
         <v>527</v>
       </c>
-      <c r="B22" s="146"/>
-      <c r="C22" s="146"/>
-      <c r="D22" s="146"/>
-      <c r="E22" s="146"/>
-      <c r="F22" s="146"/>
-      <c r="G22" s="146"/>
-      <c r="H22" s="146"/>
-      <c r="I22" s="146"/>
-      <c r="J22" s="146"/>
+      <c r="B22" s="147"/>
+      <c r="C22" s="147"/>
+      <c r="D22" s="147"/>
+      <c r="E22" s="147"/>
+      <c r="F22" s="147"/>
+      <c r="G22" s="147"/>
+      <c r="H22" s="147"/>
+      <c r="I22" s="147"/>
+      <c r="J22" s="147"/>
       <c r="K22"/>
       <c r="L22"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="131" t="s">
+    <row r="23" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="114" t="s">
         <v>528</v>
       </c>
-      <c r="B23" s="131" t="s">
+      <c r="B23" s="114" t="s">
         <v>529</v>
       </c>
-      <c r="C23" s="133">
+      <c r="C23" s="115">
         <v>42604</v>
       </c>
-      <c r="D23" s="131" t="s">
+      <c r="D23" s="114" t="s">
         <v>530</v>
       </c>
       <c r="E23" s="32" t="s">
@@ -12148,12 +12148,12 @@
       <c r="L23" s="98"/>
       <c r="M23" s="95"/>
     </row>
-    <row r="24" spans="1:13" ht="25.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="131"/>
-      <c r="B24" s="131"/>
-      <c r="C24" s="133"/>
-      <c r="D24" s="131"/>
-      <c r="E24" s="131" t="s">
+    <row r="24" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="114"/>
+      <c r="B24" s="114"/>
+      <c r="C24" s="115"/>
+      <c r="D24" s="114"/>
+      <c r="E24" s="114" t="s">
         <v>534</v>
       </c>
       <c r="F24" s="32" t="s">
@@ -12173,12 +12173,12 @@
       <c r="L24" s="98"/>
       <c r="M24" s="95"/>
     </row>
-    <row r="25" spans="1:13" ht="25.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="131"/>
-      <c r="B25" s="131"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="131"/>
-      <c r="E25" s="131"/>
+    <row r="25" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="114"/>
+      <c r="B25" s="114"/>
+      <c r="C25" s="115"/>
+      <c r="D25" s="114"/>
+      <c r="E25" s="114"/>
       <c r="F25" s="32" t="s">
         <v>536</v>
       </c>
@@ -12196,12 +12196,12 @@
       <c r="L25" s="98"/>
       <c r="M25" s="95"/>
     </row>
-    <row r="26" spans="1:13" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="131"/>
-      <c r="B26" s="131"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="131"/>
-      <c r="E26" s="131"/>
+    <row r="26" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="114"/>
+      <c r="B26" s="114"/>
+      <c r="C26" s="115"/>
+      <c r="D26" s="114"/>
+      <c r="E26" s="114"/>
       <c r="F26" s="32" t="s">
         <v>537</v>
       </c>
@@ -12219,7 +12219,7 @@
       <c r="L26" s="98"/>
       <c r="M26" s="95"/>
     </row>
-    <row r="27" spans="1:13" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="51" x14ac:dyDescent="0.25">
       <c r="A27" s="99" t="s">
         <v>538</v>
       </c>
@@ -12252,7 +12252,7 @@
       <c r="L27" s="98"/>
       <c r="M27" s="95"/>
     </row>
-    <row r="28" spans="1:13" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A28" s="40"/>
       <c r="B28" s="32"/>
       <c r="C28" s="33"/>
@@ -12279,7 +12279,7 @@
       <c r="L28" s="98"/>
       <c r="M28" s="95"/>
     </row>
-    <row r="29" spans="1:13" ht="102" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="102" x14ac:dyDescent="0.25">
       <c r="A29" s="32" t="s">
         <v>546</v>
       </c>
@@ -12312,7 +12312,7 @@
       <c r="L29" s="98"/>
       <c r="M29" s="95"/>
     </row>
-    <row r="30" spans="1:13" ht="51" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="51" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="s">
         <v>551</v>
       </c>
@@ -12374,7 +12374,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="38.25" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A32" s="102" t="s">
         <v>559</v>
       </c>
@@ -12408,13 +12408,13 @@
       </c>
     </row>
     <row r="33" spans="1:13" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="131" t="s">
+      <c r="A33" s="114" t="s">
         <v>564</v>
       </c>
-      <c r="B33" s="131" t="s">
+      <c r="B33" s="114" t="s">
         <v>565</v>
       </c>
-      <c r="C33" s="133">
+      <c r="C33" s="115">
         <v>42607</v>
       </c>
       <c r="D33" s="32" t="s">
@@ -12439,9 +12439,9 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="131"/>
-      <c r="B34" s="131"/>
-      <c r="C34" s="133"/>
+      <c r="A34" s="114"/>
+      <c r="B34" s="114"/>
+      <c r="C34" s="115"/>
       <c r="D34" s="32" t="s">
         <v>568</v>
       </c>
@@ -12462,10 +12462,10 @@
       <c r="M34" s="149"/>
     </row>
     <row r="35" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="131"/>
-      <c r="B35" s="131"/>
-      <c r="C35" s="133"/>
-      <c r="D35" s="131" t="s">
+      <c r="A35" s="114"/>
+      <c r="B35" s="114"/>
+      <c r="C35" s="115"/>
+      <c r="D35" s="114" t="s">
         <v>570</v>
       </c>
       <c r="E35" s="32" t="s">
@@ -12485,10 +12485,10 @@
       <c r="M35" s="149"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="131"/>
-      <c r="B36" s="131"/>
-      <c r="C36" s="133"/>
-      <c r="D36" s="131"/>
+      <c r="A36" s="114"/>
+      <c r="B36" s="114"/>
+      <c r="C36" s="115"/>
+      <c r="D36" s="114"/>
       <c r="E36" s="32" t="s">
         <v>572</v>
       </c>
@@ -12506,9 +12506,9 @@
       <c r="M36" s="149"/>
     </row>
     <row r="37" spans="1:13" ht="25.5" x14ac:dyDescent="0.25">
-      <c r="A37" s="131"/>
-      <c r="B37" s="131"/>
-      <c r="C37" s="133"/>
+      <c r="A37" s="114"/>
+      <c r="B37" s="114"/>
+      <c r="C37" s="115"/>
       <c r="D37" s="32"/>
       <c r="E37" s="32" t="s">
         <v>573</v>
@@ -12527,9 +12527,9 @@
       <c r="M37" s="149"/>
     </row>
     <row r="38" spans="1:13" ht="38.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="131"/>
-      <c r="B38" s="131"/>
-      <c r="C38" s="133"/>
+      <c r="A38" s="114"/>
+      <c r="B38" s="114"/>
+      <c r="C38" s="115"/>
       <c r="D38" s="32"/>
       <c r="E38" s="32" t="s">
         <v>574</v>
@@ -12573,16 +12573,16 @@
       <c r="M39" s="149"/>
     </row>
     <row r="40" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="148"/>
-      <c r="B40" s="148"/>
-      <c r="C40" s="148"/>
-      <c r="D40" s="148"/>
-      <c r="E40" s="148"/>
-      <c r="F40" s="148"/>
-      <c r="G40" s="148"/>
-      <c r="H40" s="148"/>
-      <c r="I40" s="148"/>
-      <c r="J40" s="148"/>
+      <c r="A40" s="145"/>
+      <c r="B40" s="145"/>
+      <c r="C40" s="145"/>
+      <c r="D40" s="145"/>
+      <c r="E40" s="145"/>
+      <c r="F40" s="145"/>
+      <c r="G40" s="145"/>
+      <c r="H40" s="145"/>
+      <c r="I40" s="145"/>
+      <c r="J40" s="145"/>
       <c r="K40" s="82"/>
       <c r="L40" s="82"/>
       <c r="M40" s="97"/>
@@ -12620,79 +12620,84 @@
       <c r="H43" s="3"/>
     </row>
     <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="141" t="s">
+      <c r="A44" s="111" t="s">
         <v>393</v>
       </c>
-      <c r="B44" s="144"/>
+      <c r="B44" s="118"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="141"/>
-      <c r="B45" s="144"/>
+      <c r="A45" s="111"/>
+      <c r="B45" s="118"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="141"/>
-      <c r="B46" s="144"/>
+      <c r="A46" s="111"/>
+      <c r="B46" s="118"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
     </row>
     <row r="47" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="141" t="s">
+      <c r="A47" s="111" t="s">
         <v>394</v>
       </c>
-      <c r="B47" s="142"/>
+      <c r="B47" s="112"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="141"/>
-      <c r="B48" s="142"/>
+      <c r="A48" s="111"/>
+      <c r="B48" s="112"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="141"/>
-      <c r="B49" s="142"/>
+      <c r="A49" s="111"/>
+      <c r="B49" s="112"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="141" t="s">
+      <c r="A50" s="111" t="s">
         <v>395</v>
       </c>
-      <c r="B50" s="142"/>
+      <c r="B50" s="112"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="141"/>
-      <c r="B51" s="142"/>
+      <c r="A51" s="111"/>
+      <c r="B51" s="112"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="141"/>
-      <c r="B52" s="142"/>
+      <c r="A52" s="111"/>
+      <c r="B52" s="112"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="A50:A52"/>
-    <mergeCell ref="B50:B52"/>
-    <mergeCell ref="A40:J40"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="A47:A49"/>
-    <mergeCell ref="B47:B49"/>
-    <mergeCell ref="A33:A38"/>
-    <mergeCell ref="B33:B38"/>
-    <mergeCell ref="C33:C38"/>
-    <mergeCell ref="M33:M39"/>
-    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="B1:E6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A8:F9"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A13:F13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:J18"/>
     <mergeCell ref="M19:M20"/>
     <mergeCell ref="A22:J22"/>
     <mergeCell ref="A23:A26"/>
@@ -12709,23 +12714,18 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="C18:J18"/>
-    <mergeCell ref="A10:F10"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A12:F12"/>
-    <mergeCell ref="A13:F13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A1:A6"/>
-    <mergeCell ref="B1:E6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A8:F9"/>
+    <mergeCell ref="A33:A38"/>
+    <mergeCell ref="B33:B38"/>
+    <mergeCell ref="C33:C38"/>
+    <mergeCell ref="M33:M39"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="A50:A52"/>
+    <mergeCell ref="B50:B52"/>
+    <mergeCell ref="A40:J40"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="A47:A49"/>
+    <mergeCell ref="B47:B49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>